<commit_message>
commit vehicle multi worksheet
</commit_message>
<xml_diff>
--- a/uploads/traffic_years_2554.xlsx
+++ b/uploads/traffic_years_2554.xlsx
@@ -923,72 +923,6 @@
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="33" borderId="21" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1038,6 +972,72 @@
     </xf>
     <xf numFmtId="164" fontId="19" fillId="33" borderId="27" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1385,7 +1385,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,1411 +1395,1413 @@
     <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
+    <row r="1" spans="1:28" ht="72" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
     </row>
     <row r="2" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="2" t="s">
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="26"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A3" s="7"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="22"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="5" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="5" t="s">
+      <c r="S3" s="30"/>
+      <c r="T3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="5" t="s">
+      <c r="U3" s="30"/>
+      <c r="V3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="3"/>
-      <c r="X3" s="5" t="s">
+      <c r="W3" s="30"/>
+      <c r="X3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="5" t="s">
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="14" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A4" s="21"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="22"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="26" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="26" t="s">
+      <c r="T4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="26" t="s">
+      <c r="U4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="V4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="26" t="s">
+      <c r="W4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="26" t="s">
+      <c r="X4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" s="26" t="s">
+      <c r="Y4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="26" t="s">
+      <c r="Z4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="26" t="s">
+      <c r="AA4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="17"/>
+      <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="2">
         <v>5970</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="7">
         <v>196</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="7">
         <v>48</v>
       </c>
-      <c r="E5" s="29">
-        <v>0</v>
-      </c>
-      <c r="F5" s="29">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
         <v>1400</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="7">
         <v>12</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="7">
         <v>862</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="7">
         <v>84</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="7">
         <v>927</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="7">
         <v>85</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="7">
         <v>109</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="7">
         <v>125</v>
       </c>
-      <c r="N5" s="29">
-        <v>0</v>
-      </c>
-      <c r="O5" s="29">
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
         <v>96</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5" s="7">
         <v>223</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="8">
         <v>70569348</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="9">
         <v>659</v>
       </c>
-      <c r="S5" s="31">
+      <c r="S5" s="9">
         <v>226</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="9">
         <v>217</v>
       </c>
-      <c r="U5" s="31">
+      <c r="U5" s="9">
         <v>113</v>
       </c>
-      <c r="V5" s="31">
+      <c r="V5" s="9">
         <v>692</v>
       </c>
-      <c r="W5" s="31">
+      <c r="W5" s="9">
         <v>399</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="9">
         <v>3027</v>
       </c>
-      <c r="Y5" s="31">
+      <c r="Y5" s="9">
         <v>352</v>
       </c>
-      <c r="Z5" s="31">
+      <c r="Z5" s="9">
         <v>53</v>
       </c>
-      <c r="AA5" s="31">
+      <c r="AA5" s="9">
         <v>5</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AB5" s="10">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="3">
         <v>2213</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="7">
         <v>128</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="7">
         <v>11</v>
       </c>
-      <c r="E6" s="29">
-        <v>0</v>
-      </c>
-      <c r="F6" s="29">
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
         <v>816</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="7">
         <v>9</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="7">
         <v>408</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="7">
         <v>39</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="7">
         <v>530</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="7">
         <v>46</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="7">
         <v>47</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="7">
         <v>70</v>
       </c>
-      <c r="N6" s="29">
-        <v>0</v>
-      </c>
-      <c r="O6" s="29">
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
         <v>10</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="7">
         <v>82</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="8">
         <v>40545019</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="9">
         <v>651</v>
       </c>
-      <c r="S6" s="31">
+      <c r="S6" s="9">
         <v>210</v>
       </c>
-      <c r="T6" s="31">
+      <c r="T6" s="9">
         <v>288</v>
       </c>
-      <c r="U6" s="31">
+      <c r="U6" s="9">
         <v>166</v>
       </c>
-      <c r="V6" s="31">
+      <c r="V6" s="9">
         <v>627</v>
       </c>
-      <c r="W6" s="31">
+      <c r="W6" s="9">
         <v>385</v>
       </c>
-      <c r="X6" s="31">
+      <c r="X6" s="9">
         <v>1303</v>
       </c>
-      <c r="Y6" s="31">
+      <c r="Y6" s="9">
         <v>176</v>
       </c>
-      <c r="Z6" s="31">
+      <c r="Z6" s="9">
         <v>75</v>
       </c>
-      <c r="AA6" s="31">
+      <c r="AA6" s="9">
         <v>5</v>
       </c>
-      <c r="AB6" s="32">
+      <c r="AB6" s="10">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="23.25" x14ac:dyDescent="0.5">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="3">
         <v>4267</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="7">
         <v>280</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="7">
         <v>48</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="7">
         <v>1524</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="7">
         <v>10</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="7">
         <v>542</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="7">
         <v>47</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="7">
         <v>888</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="7">
         <v>64</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="7">
         <v>109</v>
       </c>
-      <c r="M7" s="29">
+      <c r="M7" s="7">
         <v>75</v>
       </c>
-      <c r="N7" s="29">
-        <v>0</v>
-      </c>
-      <c r="O7" s="29">
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
         <v>15</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7" s="7">
         <v>175</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="Q7" s="8">
         <v>73725192</v>
       </c>
-      <c r="R7" s="31">
+      <c r="R7" s="9">
         <v>1018</v>
       </c>
-      <c r="S7" s="31">
+      <c r="S7" s="9">
         <v>321</v>
       </c>
-      <c r="T7" s="31">
+      <c r="T7" s="9">
         <v>378</v>
       </c>
-      <c r="U7" s="31">
+      <c r="U7" s="9">
         <v>204</v>
       </c>
-      <c r="V7" s="31">
+      <c r="V7" s="9">
         <v>1127</v>
       </c>
-      <c r="W7" s="31">
+      <c r="W7" s="9">
         <v>599</v>
       </c>
-      <c r="X7" s="31">
+      <c r="X7" s="9">
         <v>1757</v>
       </c>
-      <c r="Y7" s="31">
+      <c r="Y7" s="9">
         <v>252</v>
       </c>
-      <c r="Z7" s="31">
+      <c r="Z7" s="9">
         <v>53</v>
       </c>
-      <c r="AA7" s="31">
+      <c r="AA7" s="9">
         <v>2</v>
       </c>
-      <c r="AB7" s="32">
+      <c r="AB7" s="10">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="3">
         <v>2624</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="7">
         <v>226</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="7">
         <v>40</v>
       </c>
-      <c r="E8" s="29">
-        <v>0</v>
-      </c>
-      <c r="F8" s="29">
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
         <v>1044</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="7">
         <v>367</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="7">
         <v>36</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="7">
         <v>572</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="7">
         <v>42</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="7">
         <v>98</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="7">
         <v>47</v>
       </c>
-      <c r="N8" s="29">
-        <v>0</v>
-      </c>
-      <c r="O8" s="29">
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
         <v>5</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P8" s="7">
         <v>116</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="8">
         <v>68725628</v>
       </c>
-      <c r="R8" s="34">
+      <c r="R8" s="12">
         <v>1106</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="13">
         <v>320</v>
       </c>
-      <c r="T8" s="35">
+      <c r="T8" s="13">
         <v>408</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U8" s="13">
         <v>210</v>
       </c>
-      <c r="V8" s="35">
+      <c r="V8" s="13">
         <v>571</v>
       </c>
-      <c r="W8" s="35">
+      <c r="W8" s="13">
         <v>297</v>
       </c>
-      <c r="X8" s="35">
+      <c r="X8" s="13">
         <v>1536</v>
       </c>
-      <c r="Y8" s="35">
+      <c r="Y8" s="13">
         <v>204</v>
       </c>
-      <c r="Z8" s="35">
+      <c r="Z8" s="13">
         <v>79</v>
       </c>
-      <c r="AA8" s="35">
+      <c r="AA8" s="13">
         <v>4</v>
       </c>
-      <c r="AB8" s="36">
+      <c r="AB8" s="14">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="3">
         <v>7345</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="7">
         <v>145</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="7">
         <v>36</v>
       </c>
-      <c r="E9" s="29">
-        <v>0</v>
-      </c>
-      <c r="F9" s="29">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
         <v>1091</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="7">
         <v>438</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="7">
         <v>36</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="7">
         <v>629</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="7">
         <v>24</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="7">
         <v>67</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="7">
         <v>43</v>
       </c>
-      <c r="N9" s="29">
-        <v>0</v>
-      </c>
-      <c r="O9" s="29">
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
         <v>4</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9" s="7">
         <v>67</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="8">
         <v>48601053</v>
       </c>
-      <c r="R9" s="34">
+      <c r="R9" s="12">
         <v>664</v>
       </c>
-      <c r="S9" s="35">
+      <c r="S9" s="13">
         <v>227</v>
       </c>
-      <c r="T9" s="35">
+      <c r="T9" s="13">
         <v>245</v>
       </c>
-      <c r="U9" s="35">
+      <c r="U9" s="13">
         <v>119</v>
       </c>
-      <c r="V9" s="35">
+      <c r="V9" s="13">
         <v>681</v>
       </c>
-      <c r="W9" s="35">
+      <c r="W9" s="13">
         <v>376</v>
       </c>
-      <c r="X9" s="35">
+      <c r="X9" s="13">
         <v>2513</v>
       </c>
-      <c r="Y9" s="35">
+      <c r="Y9" s="13">
         <v>255</v>
       </c>
-      <c r="Z9" s="35">
+      <c r="Z9" s="13">
         <v>23</v>
       </c>
-      <c r="AA9" s="35">
+      <c r="AA9" s="13">
         <v>3</v>
       </c>
-      <c r="AB9" s="36">
+      <c r="AB9" s="14">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="3">
         <v>2532</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="7">
         <v>141</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="7">
         <v>40</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="7">
         <v>909</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="7">
         <v>5</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="7">
         <v>348</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="7">
         <v>30</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="7">
         <v>476</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="7">
         <v>27</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="7">
         <v>50</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="7">
         <v>65</v>
       </c>
-      <c r="N10" s="29">
-        <v>0</v>
-      </c>
-      <c r="O10" s="29">
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7">
         <v>2</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="7">
         <v>111</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="8">
         <v>30999139</v>
       </c>
-      <c r="R10" s="34">
+      <c r="R10" s="12">
         <v>742</v>
       </c>
-      <c r="S10" s="35">
+      <c r="S10" s="13">
         <v>267</v>
       </c>
-      <c r="T10" s="35">
+      <c r="T10" s="13">
         <v>242</v>
       </c>
-      <c r="U10" s="35">
+      <c r="U10" s="13">
         <v>118</v>
       </c>
-      <c r="V10" s="35">
+      <c r="V10" s="13">
         <v>631</v>
       </c>
-      <c r="W10" s="35">
+      <c r="W10" s="13">
         <v>385</v>
       </c>
-      <c r="X10" s="35">
+      <c r="X10" s="13">
         <v>1104</v>
       </c>
-      <c r="Y10" s="35">
+      <c r="Y10" s="13">
         <v>155</v>
       </c>
-      <c r="Z10" s="35">
+      <c r="Z10" s="13">
         <v>43</v>
       </c>
-      <c r="AA10" s="35">
+      <c r="AA10" s="13">
         <v>8</v>
       </c>
-      <c r="AB10" s="36">
+      <c r="AB10" s="14">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="3">
         <v>2002</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="7">
         <v>104</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="7">
         <v>30</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="7">
         <v>942</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="7">
         <v>3</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="7">
         <v>391</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="7">
         <v>50</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="7">
         <v>545</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="7">
         <v>19</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="7">
         <v>52</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="7">
         <v>120</v>
       </c>
-      <c r="N11" s="29">
-        <v>0</v>
-      </c>
-      <c r="O11" s="29">
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
         <v>15</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="7">
         <v>91</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="8">
         <v>138264959</v>
       </c>
-      <c r="R11" s="34">
+      <c r="R11" s="12">
         <v>597</v>
       </c>
-      <c r="S11" s="35">
+      <c r="S11" s="13">
         <v>229</v>
       </c>
-      <c r="T11" s="35">
+      <c r="T11" s="13">
         <v>241</v>
       </c>
-      <c r="U11" s="35">
+      <c r="U11" s="13">
         <v>164</v>
       </c>
-      <c r="V11" s="35">
+      <c r="V11" s="13">
         <v>544</v>
       </c>
-      <c r="W11" s="35">
+      <c r="W11" s="13">
         <v>348</v>
       </c>
-      <c r="X11" s="35">
+      <c r="X11" s="13">
         <v>946</v>
       </c>
-      <c r="Y11" s="35">
+      <c r="Y11" s="13">
         <v>142</v>
       </c>
-      <c r="Z11" s="35">
+      <c r="Z11" s="13">
         <v>46</v>
       </c>
-      <c r="AA11" s="35">
+      <c r="AA11" s="13">
         <v>6</v>
       </c>
-      <c r="AB11" s="36">
+      <c r="AB11" s="14">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="3">
         <v>4232</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="7">
         <v>187</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="7">
         <v>19</v>
       </c>
-      <c r="E12" s="29">
-        <v>0</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
         <v>1641</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="7">
         <v>615</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="7">
         <v>45</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="7">
         <v>896</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="7">
         <v>26</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="7">
         <v>77</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="7">
         <v>102</v>
       </c>
-      <c r="N12" s="29">
-        <v>0</v>
-      </c>
-      <c r="O12" s="29">
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7">
         <v>5</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12" s="7">
         <v>93</v>
       </c>
-      <c r="Q12" s="30">
+      <c r="Q12" s="8">
         <v>36056060</v>
       </c>
-      <c r="R12" s="34">
+      <c r="R12" s="12">
         <v>654</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S12" s="13">
         <v>257</v>
       </c>
-      <c r="T12" s="35">
+      <c r="T12" s="13">
         <v>250</v>
       </c>
-      <c r="U12" s="35">
+      <c r="U12" s="13">
         <v>181</v>
       </c>
-      <c r="V12" s="35">
+      <c r="V12" s="13">
         <v>1091</v>
       </c>
-      <c r="W12" s="35">
+      <c r="W12" s="13">
         <v>671</v>
       </c>
-      <c r="X12" s="35">
+      <c r="X12" s="13">
         <v>1761</v>
       </c>
-      <c r="Y12" s="35">
+      <c r="Y12" s="13">
         <v>282</v>
       </c>
-      <c r="Z12" s="35">
+      <c r="Z12" s="13">
         <v>88</v>
       </c>
-      <c r="AA12" s="35">
+      <c r="AA12" s="13">
         <v>9</v>
       </c>
-      <c r="AB12" s="36">
+      <c r="AB12" s="14">
         <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="3">
         <v>1012</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="7">
         <v>80</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="7">
         <v>11</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="7">
         <v>1</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="7">
         <v>592</v>
       </c>
-      <c r="G13" s="29">
-        <v>0</v>
-      </c>
-      <c r="H13" s="29">
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
         <v>186</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="7">
         <v>17</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="7">
         <v>323</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="7">
         <v>8</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="7">
         <v>29</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="7">
         <v>33</v>
       </c>
-      <c r="N13" s="29">
-        <v>0</v>
-      </c>
-      <c r="O13" s="29">
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
         <v>3</v>
       </c>
-      <c r="P13" s="29">
+      <c r="P13" s="7">
         <v>34</v>
       </c>
-      <c r="Q13" s="30">
+      <c r="Q13" s="8">
         <v>32665038</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="12">
         <v>394</v>
       </c>
-      <c r="S13" s="35">
+      <c r="S13" s="13">
         <v>148</v>
       </c>
-      <c r="T13" s="35">
+      <c r="T13" s="13">
         <v>155</v>
       </c>
-      <c r="U13" s="35">
+      <c r="U13" s="13">
         <v>77</v>
       </c>
-      <c r="V13" s="35">
+      <c r="V13" s="13">
         <v>323</v>
       </c>
-      <c r="W13" s="35">
+      <c r="W13" s="13">
         <v>164</v>
       </c>
-      <c r="X13" s="35">
+      <c r="X13" s="13">
         <v>543</v>
       </c>
-      <c r="Y13" s="35">
+      <c r="Y13" s="13">
         <v>73</v>
       </c>
-      <c r="Z13" s="35">
+      <c r="Z13" s="13">
         <v>45</v>
       </c>
-      <c r="AA13" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="36">
+      <c r="AA13" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="14">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="3">
         <v>438</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="7">
         <v>52</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="7">
         <v>6</v>
       </c>
-      <c r="E14" s="29">
-        <v>0</v>
-      </c>
-      <c r="F14" s="29">
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
         <v>183</v>
       </c>
-      <c r="G14" s="29">
-        <v>0</v>
-      </c>
-      <c r="H14" s="29">
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
         <v>76</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="7">
         <v>9</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="7">
         <v>87</v>
       </c>
-      <c r="K14" s="29">
-        <v>0</v>
-      </c>
-      <c r="L14" s="29">
+      <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
         <v>8</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="7">
         <v>8</v>
       </c>
-      <c r="N14" s="29">
-        <v>0</v>
-      </c>
-      <c r="O14" s="29">
-        <v>0</v>
-      </c>
-      <c r="P14" s="29">
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
         <v>4</v>
       </c>
-      <c r="Q14" s="30">
+      <c r="Q14" s="8">
         <v>1116116</v>
       </c>
-      <c r="R14" s="34">
+      <c r="R14" s="12">
         <v>96</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S14" s="13">
         <v>59</v>
       </c>
-      <c r="T14" s="35">
+      <c r="T14" s="13">
         <v>35</v>
       </c>
-      <c r="U14" s="35">
+      <c r="U14" s="13">
         <v>23</v>
       </c>
-      <c r="V14" s="35">
+      <c r="V14" s="13">
         <v>136</v>
       </c>
-      <c r="W14" s="35">
+      <c r="W14" s="13">
         <v>112</v>
       </c>
-      <c r="X14" s="35">
+      <c r="X14" s="13">
         <v>164</v>
       </c>
-      <c r="Y14" s="35">
+      <c r="Y14" s="13">
         <v>31</v>
       </c>
-      <c r="Z14" s="35">
+      <c r="Z14" s="13">
         <v>5</v>
       </c>
-      <c r="AA14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="36">
+      <c r="AA14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="3">
         <v>35703</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="7">
         <v>1102</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="7">
         <v>116</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="7">
         <v>16</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="7">
         <v>9954</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="7">
         <v>197</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="7">
         <v>12390</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="7">
         <v>521</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="7">
         <v>3214</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="7">
         <v>649</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="7">
         <v>387</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="7">
         <v>319</v>
       </c>
-      <c r="N15" s="29">
-        <v>0</v>
-      </c>
-      <c r="O15" s="29">
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
         <v>2874</v>
       </c>
-      <c r="P15" s="29">
+      <c r="P15" s="7">
         <v>373</v>
       </c>
-      <c r="Q15" s="30">
+      <c r="Q15" s="8">
         <v>80899423</v>
       </c>
-      <c r="R15" s="34">
+      <c r="R15" s="12">
         <v>269</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="13">
         <v>76</v>
       </c>
-      <c r="T15" s="35">
+      <c r="T15" s="13">
         <v>168</v>
       </c>
-      <c r="U15" s="35">
+      <c r="U15" s="13">
         <v>90</v>
       </c>
-      <c r="V15" s="35">
+      <c r="V15" s="13">
         <v>4816</v>
       </c>
-      <c r="W15" s="35">
+      <c r="W15" s="13">
         <v>2839</v>
       </c>
-      <c r="X15" s="35">
+      <c r="X15" s="13">
         <v>21470</v>
       </c>
-      <c r="Y15" s="35">
+      <c r="Y15" s="13">
         <v>2883</v>
       </c>
-      <c r="Z15" s="35">
+      <c r="Z15" s="13">
         <v>55</v>
       </c>
-      <c r="AA15" s="35">
+      <c r="AA15" s="13">
         <v>2</v>
       </c>
-      <c r="AB15" s="36">
+      <c r="AB15" s="14">
         <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="3">
         <v>244</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="7">
         <v>3</v>
       </c>
-      <c r="D16" s="29">
-        <v>0</v>
-      </c>
-      <c r="E16" s="29">
-        <v>0</v>
-      </c>
-      <c r="F16" s="29">
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
         <v>5</v>
       </c>
-      <c r="G16" s="29">
-        <v>0</v>
-      </c>
-      <c r="H16" s="29">
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
         <v>10</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="7">
         <v>2</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="7">
         <v>24</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="7">
         <v>1</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="7">
         <v>1</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="7">
         <v>1</v>
       </c>
-      <c r="N16" s="29">
-        <v>0</v>
-      </c>
-      <c r="O16" s="29">
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
         <v>3</v>
       </c>
-      <c r="P16" s="29">
+      <c r="P16" s="7">
         <v>5</v>
       </c>
-      <c r="Q16" s="30">
-        <v>0</v>
-      </c>
-      <c r="R16" s="34">
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="R16" s="12">
         <v>8</v>
       </c>
-      <c r="S16" s="35">
+      <c r="S16" s="13">
         <v>7</v>
       </c>
-      <c r="T16" s="35">
-        <v>0</v>
-      </c>
-      <c r="U16" s="35">
+      <c r="T16" s="13">
+        <v>0</v>
+      </c>
+      <c r="U16" s="13">
         <v>1</v>
       </c>
-      <c r="V16" s="35">
+      <c r="V16" s="13">
         <v>4</v>
       </c>
-      <c r="W16" s="35">
+      <c r="W16" s="13">
         <v>5</v>
       </c>
-      <c r="X16" s="35">
+      <c r="X16" s="13">
         <v>112</v>
       </c>
-      <c r="Y16" s="35">
+      <c r="Y16" s="13">
         <v>10</v>
       </c>
-      <c r="Z16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="36">
+      <c r="Z16" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="14">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="29">
-        <v>0</v>
-      </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="29">
-        <v>0</v>
-      </c>
-      <c r="F17" s="29">
-        <v>0</v>
-      </c>
-      <c r="G17" s="29">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29">
-        <v>0</v>
-      </c>
-      <c r="I17" s="29">
-        <v>0</v>
-      </c>
-      <c r="J17" s="29">
-        <v>0</v>
-      </c>
-      <c r="K17" s="29">
-        <v>0</v>
-      </c>
-      <c r="L17" s="29">
-        <v>0</v>
-      </c>
-      <c r="M17" s="29">
-        <v>0</v>
-      </c>
-      <c r="N17" s="29">
-        <v>0</v>
-      </c>
-      <c r="O17" s="29">
-        <v>0</v>
-      </c>
-      <c r="P17" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>0</v>
-      </c>
-      <c r="R17" s="34">
-        <v>0</v>
-      </c>
-      <c r="S17" s="35">
-        <v>0</v>
-      </c>
-      <c r="T17" s="35">
-        <v>0</v>
-      </c>
-      <c r="U17" s="35">
-        <v>0</v>
-      </c>
-      <c r="V17" s="35">
-        <v>0</v>
-      </c>
-      <c r="W17" s="35">
-        <v>0</v>
-      </c>
-      <c r="X17" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="36">
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0</v>
+      </c>
+      <c r="S17" s="13">
+        <v>0</v>
+      </c>
+      <c r="T17" s="13">
+        <v>0</v>
+      </c>
+      <c r="U17" s="13">
+        <v>0</v>
+      </c>
+      <c r="V17" s="13">
+        <v>0</v>
+      </c>
+      <c r="W17" s="13">
+        <v>0</v>
+      </c>
+      <c r="X17" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="3">
         <v>68538</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="7">
         <v>2644</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="7">
         <v>405</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="7">
         <v>20</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="7">
         <v>20101</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="7">
         <v>255</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="7">
         <v>16633</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="7">
         <v>916</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="7">
         <v>9111</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="7">
         <v>991</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="7">
         <v>1034</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="7">
         <v>1008</v>
       </c>
-      <c r="N18" s="29">
-        <v>0</v>
-      </c>
-      <c r="O18" s="29">
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
         <v>3032</v>
       </c>
-      <c r="P18" s="29">
+      <c r="P18" s="7">
         <v>1374</v>
       </c>
-      <c r="Q18" s="30">
+      <c r="Q18" s="8">
         <v>622166974</v>
       </c>
-      <c r="R18" s="38">
+      <c r="R18" s="16">
         <v>6858</v>
       </c>
-      <c r="S18" s="39" t="s">
+      <c r="S18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="T18" s="40">
+      <c r="T18" s="18">
         <v>2627</v>
       </c>
-      <c r="U18" s="40">
+      <c r="U18" s="18">
         <v>1466</v>
       </c>
-      <c r="V18" s="40">
+      <c r="V18" s="18">
         <v>11243</v>
       </c>
-      <c r="W18" s="40">
+      <c r="W18" s="18">
         <v>6580</v>
       </c>
-      <c r="X18" s="40">
+      <c r="X18" s="18">
         <v>36236</v>
       </c>
-      <c r="Y18" s="40">
+      <c r="Y18" s="18">
         <v>4815</v>
       </c>
-      <c r="Z18" s="40">
+      <c r="Z18" s="18">
         <v>565</v>
       </c>
-      <c r="AA18" s="40">
+      <c r="AA18" s="18">
         <v>44</v>
       </c>
-      <c r="AB18" s="40">
+      <c r="AB18" s="18">
         <v>1132</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
     <mergeCell ref="AB3:AB4"/>
     <mergeCell ref="P2:P4"/>
     <mergeCell ref="Q2:Q4"/>
@@ -2810,15 +2812,13 @@
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>